<commit_message>
comenzamos con el loader
</commit_message>
<xml_diff>
--- a/Analisis/Mercancias.xlsx
+++ b/Analisis/Mercancias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC79473-A184-413E-BEE5-5BB60A1601B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BEC5791-E744-49A9-9078-91A106A6BFC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{EC70344D-1429-4290-A8D2-109C16EB33D2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="69">
   <si>
     <t>Sucursal</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>mac-adress</t>
+  </si>
+  <si>
+    <t>ventas</t>
   </si>
 </sst>
 </file>
@@ -296,9 +299,6 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -307,10 +307,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF38020E-0031-4721-8C62-05BE7B6A2264}">
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33:M33"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,44 +649,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -794,14 +797,14 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="5"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I9" t="s">
@@ -836,11 +839,11 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
       <c r="I10">
         <v>1</v>
       </c>
@@ -870,13 +873,13 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>25</v>
       </c>
       <c r="I11">
@@ -899,13 +902,13 @@
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>1</v>
-      </c>
-      <c r="B12" s="6">
+      <c r="A12" s="5">
+        <v>1</v>
+      </c>
+      <c r="B12" s="5">
         <v>97</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>85</v>
       </c>
       <c r="I12">
@@ -925,13 +928,13 @@
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>2</v>
       </c>
       <c r="B13">
         <v>100</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>25</v>
       </c>
       <c r="I13">
@@ -951,24 +954,24 @@
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>3</v>
       </c>
       <c r="B14">
         <v>10</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>4</v>
       </c>
       <c r="B15">
         <v>15</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>89</v>
       </c>
     </row>
@@ -979,59 +982,59 @@
       <c r="B16">
         <v>20</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16" s="5">
         <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="I19" s="1" t="s">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="I19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="I20" s="4" t="s">
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="I20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J20" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K20" s="4" t="s">
+      <c r="J20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L20" s="4" t="s">
+      <c r="L20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M20" s="4" t="s">
+      <c r="M20" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1039,10 +1042,10 @@
       <c r="A21">
         <v>1</v>
       </c>
-      <c r="B21" s="6">
-        <v>1</v>
-      </c>
-      <c r="C21" s="6">
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5">
         <v>97</v>
       </c>
       <c r="D21">
@@ -1054,7 +1057,7 @@
       <c r="I21">
         <v>1</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="6">
         <v>4</v>
       </c>
       <c r="K21">
@@ -1071,10 +1074,10 @@
       <c r="A22">
         <v>2</v>
       </c>
-      <c r="B22" s="6">
-        <v>2</v>
-      </c>
-      <c r="C22" s="6">
+      <c r="B22" s="5">
+        <v>2</v>
+      </c>
+      <c r="C22" s="5">
         <v>97</v>
       </c>
       <c r="D22">
@@ -1100,10 +1103,10 @@
       <c r="A23">
         <v>3</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>3</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>10</v>
       </c>
       <c r="D23">
@@ -1129,10 +1132,10 @@
       <c r="A24">
         <v>4</v>
       </c>
-      <c r="B24" s="6">
-        <v>4</v>
-      </c>
-      <c r="C24" s="6">
+      <c r="B24" s="5">
+        <v>4</v>
+      </c>
+      <c r="C24" s="5">
         <v>15</v>
       </c>
       <c r="D24">
@@ -1158,10 +1161,10 @@
       <c r="A25">
         <v>5</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>5</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>20</v>
       </c>
       <c r="D25">
@@ -1187,10 +1190,10 @@
       <c r="A26">
         <v>6</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>6</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="5">
         <v>97</v>
       </c>
       <c r="D26">
@@ -1199,7 +1202,7 @@
       <c r="I26">
         <v>6</v>
       </c>
-      <c r="J26" s="7">
+      <c r="J26" s="6">
         <v>2</v>
       </c>
       <c r="K26">
@@ -1216,10 +1219,10 @@
       <c r="A27">
         <v>7</v>
       </c>
-      <c r="B27" s="6">
-        <v>1</v>
-      </c>
-      <c r="C27" s="6">
+      <c r="B27" s="5">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5">
         <v>98</v>
       </c>
       <c r="D27">
@@ -1245,10 +1248,10 @@
       <c r="A28">
         <v>8</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <v>8</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="5">
         <v>105</v>
       </c>
       <c r="D28">
@@ -1274,10 +1277,10 @@
       <c r="A29">
         <v>9</v>
       </c>
-      <c r="B29" s="6">
-        <v>1</v>
-      </c>
-      <c r="C29" s="6">
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5">
         <v>90</v>
       </c>
       <c r="D29">
@@ -1303,19 +1306,19 @@
       <c r="A30">
         <v>10</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <v>10</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="5">
         <v>97</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <v>30</v>
       </c>
       <c r="I30">
         <v>10</v>
       </c>
-      <c r="J30" s="7">
+      <c r="J30" s="6">
         <v>1</v>
       </c>
       <c r="K30">
@@ -1329,77 +1332,77 @@
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="K33" s="1" t="s">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="K33" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
+      <c r="L33" s="8"/>
+      <c r="M33" s="8"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="7" t="s">
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="L34" s="7" t="s">
+      <c r="L34" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="M34" s="7" t="s">
+      <c r="M34" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="G35" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="H35" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I35" s="4" t="s">
+      <c r="I35" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="J35" s="4" t="s">
+      <c r="J35" s="3" t="s">
         <v>31</v>
       </c>
       <c r="K35">
@@ -1467,7 +1470,7 @@
         <v>5</v>
       </c>
       <c r="F37">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G37">
         <v>100</v>
@@ -1510,22 +1513,28 @@
       <c r="H38">
         <v>585659</v>
       </c>
-      <c r="I38" s="9">
+      <c r="I38" s="7">
         <v>43925</v>
       </c>
       <c r="J38">
         <v>1</v>
       </c>
+      <c r="K38">
+        <v>4</v>
+      </c>
+      <c r="L38" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
@@ -1574,16 +1583,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="I19:M19"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="K33:M33"/>
     <mergeCell ref="I8:M8"/>
     <mergeCell ref="A40:H40"/>
     <mergeCell ref="A34:J34"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="A19:G19"/>
-    <mergeCell ref="I19:M19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adecuaciones a las tablas para el registro
</commit_message>
<xml_diff>
--- a/Analisis/Mercancias.xlsx
+++ b/Analisis/Mercancias.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victor/Documents/Proyectos Web/comercializadora/Analisis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{245B26BE-F64A-2D44-B6D1-6044EA257683}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCEADF4-41FE-45E7-843D-5786E2EC9695}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20640" windowHeight="11320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="106">
   <si>
     <t>Sucursal</t>
   </si>
@@ -112,33 +112,9 @@
     <t>id</t>
   </si>
   <si>
-    <t>IdAlmacen</t>
-  </si>
-  <si>
-    <t>Pasillo</t>
-  </si>
-  <si>
-    <t>Piso</t>
-  </si>
-  <si>
-    <t>operación</t>
-  </si>
-  <si>
     <t>Inventario General</t>
   </si>
   <si>
-    <t>usuario logueado</t>
-  </si>
-  <si>
-    <t>IdAlmacen Destino</t>
-  </si>
-  <si>
-    <t>raq</t>
-  </si>
-  <si>
-    <t>descripcion</t>
-  </si>
-  <si>
     <t>Estatus</t>
   </si>
   <si>
@@ -214,12 +190,6 @@
     <t>IdInventarioDetalleLog</t>
   </si>
   <si>
-    <t>Realizar Pedido</t>
-  </si>
-  <si>
-    <t>Pedido Recibido</t>
-  </si>
-  <si>
     <t>PedidosInternos</t>
   </si>
   <si>
@@ -241,18 +211,12 @@
     <t>IdPedidoInternoDetalle</t>
   </si>
   <si>
-    <t>IdEstatus</t>
-  </si>
-  <si>
     <t>CatEstatusPedidInterno</t>
   </si>
   <si>
     <t>PedidoRealizado</t>
   </si>
   <si>
-    <t>PedidoEnviado</t>
-  </si>
-  <si>
     <t>PedidoFinalizado</t>
   </si>
   <si>
@@ -265,9 +229,6 @@
     <t>IventarioDetalleLog</t>
   </si>
   <si>
-    <t>TipoMov</t>
-  </si>
-  <si>
     <t>Venta</t>
   </si>
   <si>
@@ -277,18 +238,6 @@
     <t>Cancelacion</t>
   </si>
   <si>
-    <t>Pedido Finalizado</t>
-  </si>
-  <si>
-    <t>PedidoCancelado</t>
-  </si>
-  <si>
-    <t>CatTipoMoviemintoMercancia</t>
-  </si>
-  <si>
-    <t>idTIpoMovMercancia</t>
-  </si>
-  <si>
     <t>16 de abril</t>
   </si>
   <si>
@@ -319,9 +268,6 @@
     <t>25 de abril</t>
   </si>
   <si>
-    <t>Compra Proveedor</t>
-  </si>
-  <si>
     <t>26 de abril</t>
   </si>
   <si>
@@ -356,6 +302,48 @@
   </si>
   <si>
     <t>Actualizar Ubicación (idUbuacion, x,y,z)</t>
+  </si>
+  <si>
+    <t>cantidadActual</t>
+  </si>
+  <si>
+    <t>Carga  Inventario</t>
+  </si>
+  <si>
+    <t>venta</t>
+  </si>
+  <si>
+    <t>resutir</t>
+  </si>
+  <si>
+    <t>idTipoMovInventario</t>
+  </si>
+  <si>
+    <t>CatTipoMovimientoInventario</t>
+  </si>
+  <si>
+    <t>idTipoMovInvenario</t>
+  </si>
+  <si>
+    <t>IdEstatusPeidoInterno</t>
+  </si>
+  <si>
+    <t>IdEstatusPedidoInterno</t>
+  </si>
+  <si>
+    <t>se levanta pedido</t>
+  </si>
+  <si>
+    <t>se atiende el pediddo (se despacha)</t>
+  </si>
+  <si>
+    <t>se termina el pedido en este caso se carga al inventario</t>
+  </si>
+  <si>
+    <t>se cancela el pedido siempre y cuando este no este en estatus de enviada</t>
+  </si>
+  <si>
+    <t>PedidoEnviado ó Atendido</t>
   </si>
 </sst>
 </file>
@@ -377,7 +365,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -408,6 +396,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -421,7 +415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -449,6 +443,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -765,47 +769,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U72"/>
+  <dimension ref="A1:V72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:A72"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49:J52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="18.33203125" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" customWidth="1"/>
-    <col min="12" max="12" width="20.1640625" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="18.28515625" customWidth="1"/>
+    <col min="11" max="11" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="D1" s="11" t="s">
+      <c r="B1" s="15"/>
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
       <c r="J1" s="9"/>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="11"/>
-    </row>
-    <row r="2" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="N1" s="15"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -827,14 +834,14 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="N2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -853,14 +860,14 @@
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -879,14 +886,14 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="M4">
+        <v>2</v>
+      </c>
+      <c r="N4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -905,19 +912,19 @@
       <c r="G5">
         <v>1</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>3</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -926,12 +933,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -940,77 +947,75 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="L8" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="4"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="L9" t="s">
-        <v>54</v>
-      </c>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="M8" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="4"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M9" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="N9" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="O9" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="P9" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="Q9" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="R9" t="s">
         <v>47</v>
       </c>
       <c r="S9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="T9" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="U9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="E10" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+        <v>40</v>
+      </c>
+      <c r="V9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="E10" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
       <c r="J10" s="9"/>
       <c r="K10" s="4"/>
-      <c r="L10">
-        <v>1</v>
-      </c>
+      <c r="L10" s="4"/>
       <c r="M10">
-        <v>4</v>
-      </c>
-      <c r="N10" t="s">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>4</v>
       </c>
       <c r="O10" t="s">
-        <v>56</v>
-      </c>
-      <c r="P10">
-        <v>1</v>
+        <v>52</v>
+      </c>
+      <c r="P10" t="s">
+        <v>48</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -1019,13 +1024,16 @@
         <v>1</v>
       </c>
       <c r="S10">
-        <v>2</v>
-      </c>
-      <c r="U10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>2</v>
+      </c>
+      <c r="V10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>27</v>
       </c>
@@ -1036,9 +1044,9 @@
         <v>25</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="17" t="s">
         <v>24</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -1048,34 +1056,37 @@
         <v>19</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>51</v>
+        <v>92</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="L11">
-        <v>2</v>
+        <v>32</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="M11">
-        <v>4</v>
-      </c>
-      <c r="O11" t="s">
-        <v>58</v>
-      </c>
-      <c r="P11">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>4</v>
+      </c>
+      <c r="P11" t="s">
+        <v>50</v>
       </c>
       <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11">
         <v>0</v>
       </c>
-      <c r="U11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>1</v>
       </c>
@@ -1088,26 +1099,32 @@
       <c r="E12">
         <v>1</v>
       </c>
+      <c r="H12">
+        <v>5</v>
+      </c>
+      <c r="I12">
+        <v>60</v>
+      </c>
       <c r="K12" t="s">
-        <v>80</v>
-      </c>
-      <c r="L12">
+        <v>67</v>
+      </c>
+      <c r="M12">
         <v>3</v>
       </c>
-      <c r="M12">
-        <v>4</v>
-      </c>
-      <c r="O12" t="s">
-        <v>57</v>
-      </c>
-      <c r="P12">
+      <c r="N12">
+        <v>4</v>
+      </c>
+      <c r="P12" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q12">
         <v>3</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>2</v>
       </c>
@@ -1120,26 +1137,32 @@
       <c r="E13">
         <v>2</v>
       </c>
+      <c r="H13">
+        <v>6</v>
+      </c>
+      <c r="I13">
+        <v>66</v>
+      </c>
       <c r="K13" t="s">
-        <v>81</v>
-      </c>
-      <c r="L13">
-        <v>4</v>
+        <v>68</v>
       </c>
       <c r="M13">
         <v>4</v>
       </c>
-      <c r="O13" t="s">
-        <v>59</v>
-      </c>
-      <c r="P13">
-        <v>4</v>
+      <c r="N13">
+        <v>4</v>
+      </c>
+      <c r="P13" t="s">
+        <v>51</v>
       </c>
       <c r="Q13">
+        <v>4</v>
+      </c>
+      <c r="R13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>3</v>
       </c>
@@ -1152,11 +1175,17 @@
       <c r="E14">
         <v>3</v>
       </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>67</v>
+      </c>
       <c r="K14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>4</v>
       </c>
@@ -1169,11 +1198,17 @@
       <c r="E15">
         <v>4</v>
       </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
+      <c r="I15">
+        <v>72</v>
+      </c>
       <c r="K15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1184,28 +1219,53 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M17" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M18" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="N18" t="s">
+        <v>94</v>
+      </c>
+      <c r="O18">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
       <c r="F19" s="10"/>
-      <c r="G19" s="11" t="s">
+      <c r="G19" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="11"/>
+      <c r="N19" t="s">
+        <v>95</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="17" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1215,7 +1275,7 @@
         <v>19</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="3" t="s">
@@ -1233,8 +1293,15 @@
       <c r="K20" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" s="3"/>
+      <c r="N20" t="s">
+        <v>69</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1245,12 +1312,12 @@
         <v>97</v>
       </c>
       <c r="D21">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
-      </c>
-      <c r="G21">
+        <v>44</v>
+      </c>
+      <c r="G21" s="17">
         <v>1</v>
       </c>
       <c r="H21" s="6">
@@ -1265,8 +1332,14 @@
       <c r="K21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="N21" t="s">
+        <v>93</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1280,7 +1353,7 @@
         <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="G22">
         <v>2</v>
@@ -1298,7 +1371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1312,7 +1385,7 @@
         <v>30</v>
       </c>
       <c r="E23" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="G23">
         <v>3</v>
@@ -1330,7 +1403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>4</v>
       </c>
@@ -1344,7 +1417,7 @@
         <v>89</v>
       </c>
       <c r="E24" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="G24">
         <v>4</v>
@@ -1362,7 +1435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5</v>
       </c>
@@ -1376,7 +1449,7 @@
         <v>150</v>
       </c>
       <c r="E25" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="G25">
         <v>5</v>
@@ -1394,7 +1467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>6</v>
       </c>
@@ -1408,7 +1481,7 @@
         <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="G26">
         <v>6</v>
@@ -1426,7 +1499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1440,7 +1513,7 @@
         <v>65</v>
       </c>
       <c r="E27" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="G27">
         <v>7</v>
@@ -1458,7 +1531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>8</v>
       </c>
@@ -1472,7 +1545,7 @@
         <v>100</v>
       </c>
       <c r="E28" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="G28">
         <v>8</v>
@@ -1490,7 +1563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>9</v>
       </c>
@@ -1504,7 +1577,7 @@
         <v>50</v>
       </c>
       <c r="E29" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="G29">
         <v>9</v>
@@ -1522,7 +1595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>10</v>
       </c>
@@ -1536,7 +1609,7 @@
         <v>30</v>
       </c>
       <c r="E30" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="G30">
         <v>10</v>
@@ -1554,7 +1627,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>11</v>
       </c>
@@ -1568,7 +1641,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="G31">
         <v>11</v>
@@ -1586,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>12</v>
       </c>
@@ -1600,54 +1673,40 @@
         <v>25</v>
       </c>
       <c r="E32" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="N33" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="10"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="11"/>
       <c r="M34" s="10"/>
-      <c r="N34" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="O34" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="P34" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>18</v>
@@ -1655,32 +1714,18 @@
       <c r="E35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>86</v>
+      <c r="F35" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N35">
-        <v>1</v>
-      </c>
-      <c r="O35" t="s">
-        <v>62</v>
-      </c>
-      <c r="P35">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -1697,28 +1742,16 @@
         <v>5</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G36">
-        <v>100</v>
+        <v>66480</v>
       </c>
       <c r="H36">
-        <v>66480</v>
-      </c>
-      <c r="J36">
-        <v>-1</v>
-      </c>
-      <c r="N36">
-        <v>2</v>
-      </c>
-      <c r="O36" t="s">
-        <v>63</v>
-      </c>
-      <c r="P36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -1735,25 +1768,16 @@
         <v>5</v>
       </c>
       <c r="F37">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="G37">
-        <v>100</v>
+        <v>48066</v>
       </c>
       <c r="H37">
-        <v>48066</v>
-      </c>
-      <c r="J37">
-        <v>1</v>
-      </c>
-      <c r="N37">
-        <v>3</v>
-      </c>
-      <c r="O37" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>3</v>
       </c>
@@ -1770,91 +1794,82 @@
         <v>10</v>
       </c>
       <c r="F38">
-        <v>3</v>
+        <v>1001</v>
       </c>
       <c r="G38">
-        <v>1001</v>
-      </c>
-      <c r="H38">
         <v>585659</v>
       </c>
-      <c r="I38" s="7">
-        <v>43925</v>
-      </c>
-      <c r="J38">
-        <v>1</v>
-      </c>
-      <c r="N38">
-        <v>4</v>
-      </c>
-      <c r="O38" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="12"/>
-      <c r="K40" s="12"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="H41" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H38" s="7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="16"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="12"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="H41" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="J42" s="3"/>
       <c r="K42" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="L42" s="3" t="s">
+      <c r="L42" s="3"/>
+      <c r="M42" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>100</v>
       </c>
@@ -1864,213 +1879,207 @@
       <c r="C43">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="F43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A48" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="H48" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="I48" s="11"/>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="15"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15"/>
+      <c r="H48" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="I48" s="18"/>
       <c r="J48" s="9"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
-        <v>65</v>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>71</v>
+        <v>57</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>100</v>
       </c>
       <c r="H49">
         <v>1</v>
       </c>
       <c r="I49" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+      <c r="J49" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>1</v>
+      </c>
       <c r="H50">
         <v>2</v>
       </c>
       <c r="I50" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="J50" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>2</v>
+      </c>
       <c r="H51">
         <v>3</v>
       </c>
       <c r="I51" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+      <c r="J51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>3</v>
+      </c>
       <c r="H52">
         <v>4</v>
       </c>
       <c r="I52" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
-        <v>28</v>
-      </c>
-      <c r="C54">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
-        <v>34</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
-        <v>29</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
-        <v>35</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
-        <v>30</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="J52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="14" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="B61" s="14"/>
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="B66" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="14" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="B68" s="14"/>
       <c r="C68" s="14"/>
       <c r="D68" s="14"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="M8:Q8"/>
+    <mergeCell ref="A40:K40"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="M17:O17"/>
     <mergeCell ref="A61:E61"/>
     <mergeCell ref="A68:D68"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="M1:N1"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="G19:K19"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="N33:P33"/>
-    <mergeCell ref="L8:P8"/>
-    <mergeCell ref="A40:K40"/>
-    <mergeCell ref="E10:I10"/>
-    <mergeCell ref="A19:E19"/>
     <mergeCell ref="A41:F41"/>
-    <mergeCell ref="H41:L41"/>
+    <mergeCell ref="H41:M41"/>
     <mergeCell ref="H48:I48"/>
     <mergeCell ref="A48:F48"/>
-    <mergeCell ref="A34:K34"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2085,7 +2094,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se sube mercancias.xls de como quedaron las tablas
</commit_message>
<xml_diff>
--- a/Analisis/Mercancias.xlsx
+++ b/Analisis/Mercancias.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\comer\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCEADF4-41FE-45E7-843D-5786E2EC9695}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA4EF01-32AA-4C73-8DBA-1646A579C637}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="105">
   <si>
     <t>Sucursal</t>
   </si>
@@ -203,9 +203,6 @@
   </si>
   <si>
     <t>PedidosInternosDetalle</t>
-  </si>
-  <si>
-    <t>contador</t>
   </si>
   <si>
     <t>IdPedidoInternoDetalle</t>
@@ -442,16 +439,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -771,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49:J52"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,7 +993,7 @@
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="E10" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
@@ -1046,7 +1043,7 @@
       <c r="E11" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="14" t="s">
         <v>24</v>
       </c>
       <c r="G11" s="3" t="s">
@@ -1056,13 +1053,13 @@
         <v>19</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="17" t="s">
-        <v>96</v>
+      <c r="K11" s="14" t="s">
+        <v>95</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>43</v>
@@ -1106,7 +1103,7 @@
         <v>60</v>
       </c>
       <c r="K12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M12">
         <v>3</v>
@@ -1144,7 +1141,7 @@
         <v>66</v>
       </c>
       <c r="K13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M13">
         <v>4</v>
@@ -1182,7 +1179,7 @@
         <v>67</v>
       </c>
       <c r="K14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -1205,7 +1202,7 @@
         <v>72</v>
       </c>
       <c r="K15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -1221,17 +1218,17 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="M17" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N17" s="15"/>
       <c r="O17" s="15"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M18" s="17" t="s">
-        <v>98</v>
+      <c r="M18" s="14" t="s">
+        <v>97</v>
       </c>
       <c r="N18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O18">
         <v>-1</v>
@@ -1255,7 +1252,7 @@
       <c r="K19" s="15"/>
       <c r="L19" s="11"/>
       <c r="N19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O19">
         <v>1</v>
@@ -1265,7 +1262,7 @@
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="14" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1295,7 +1292,7 @@
       </c>
       <c r="L20" s="3"/>
       <c r="N20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O20">
         <v>1</v>
@@ -1317,7 +1314,7 @@
       <c r="E21" t="s">
         <v>44</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G21" s="14">
         <v>1</v>
       </c>
       <c r="H21" s="6">
@@ -1333,7 +1330,7 @@
         <v>1</v>
       </c>
       <c r="N21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O21">
         <v>1</v>
@@ -1353,7 +1350,7 @@
         <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G22">
         <v>2</v>
@@ -1385,7 +1382,7 @@
         <v>30</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G23">
         <v>3</v>
@@ -1417,7 +1414,7 @@
         <v>89</v>
       </c>
       <c r="E24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G24">
         <v>4</v>
@@ -1449,7 +1446,7 @@
         <v>150</v>
       </c>
       <c r="E25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G25">
         <v>5</v>
@@ -1481,7 +1478,7 @@
         <v>5</v>
       </c>
       <c r="E26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G26">
         <v>6</v>
@@ -1513,7 +1510,7 @@
         <v>65</v>
       </c>
       <c r="E27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G27">
         <v>7</v>
@@ -1545,7 +1542,7 @@
         <v>100</v>
       </c>
       <c r="E28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G28">
         <v>8</v>
@@ -1577,7 +1574,7 @@
         <v>50</v>
       </c>
       <c r="E29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G29">
         <v>9</v>
@@ -1609,7 +1606,7 @@
         <v>30</v>
       </c>
       <c r="E30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G30">
         <v>10</v>
@@ -1641,7 +1638,7 @@
         <v>10</v>
       </c>
       <c r="E31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G31">
         <v>11</v>
@@ -1673,7 +1670,7 @@
         <v>25</v>
       </c>
       <c r="E32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
@@ -1714,7 +1711,7 @@
       <c r="E35" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="17" t="s">
+      <c r="F35" s="14" t="s">
         <v>55</v>
       </c>
       <c r="G35" s="3" t="s">
@@ -1852,13 +1849,13 @@
         <v>57</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>59</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="J42" s="3"/>
       <c r="K42" s="3" t="s">
@@ -1895,7 +1892,7 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B48" s="15"/>
       <c r="C48" s="15"/>
@@ -1903,13 +1900,13 @@
       <c r="E48" s="15"/>
       <c r="F48" s="15"/>
       <c r="H48" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I48" s="18"/>
       <c r="J48" s="9"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="14" t="s">
         <v>55</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -1924,17 +1921,17 @@
       <c r="E49" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F49" s="17" t="s">
+      <c r="F49" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49" t="s">
+        <v>61</v>
+      </c>
+      <c r="J49" t="s">
         <v>100</v>
-      </c>
-      <c r="H49">
-        <v>1</v>
-      </c>
-      <c r="I49" t="s">
-        <v>62</v>
-      </c>
-      <c r="J49" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
@@ -1945,10 +1942,10 @@
         <v>2</v>
       </c>
       <c r="I50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -1959,10 +1956,10 @@
         <v>3</v>
       </c>
       <c r="I51" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -1973,10 +1970,10 @@
         <v>4</v>
       </c>
       <c r="I52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -1995,13 +1992,13 @@
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A61" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
+      <c r="A61" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B61" s="17"/>
+      <c r="C61" s="17"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="13"/>
@@ -2012,63 +2009,57 @@
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B66" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="17" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="B68" s="14"/>
-      <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
+      <c r="B68" s="17"/>
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="M8:Q8"/>
-    <mergeCell ref="A40:K40"/>
-    <mergeCell ref="E10:I10"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="M17:O17"/>
     <mergeCell ref="A61:E61"/>
     <mergeCell ref="A68:D68"/>
     <mergeCell ref="A1:B1"/>
@@ -2080,6 +2071,12 @@
     <mergeCell ref="H41:M41"/>
     <mergeCell ref="H48:I48"/>
     <mergeCell ref="A48:F48"/>
+    <mergeCell ref="M8:Q8"/>
+    <mergeCell ref="A40:K40"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A34:K34"/>
+    <mergeCell ref="M17:O17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>